<commit_message>
fix data, but vse ploho with Uвых = f(Iн)
</commit_message>
<xml_diff>
--- a/lab11a/lab11a.xlsx
+++ b/lab11a/lab11a.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="U = f(U)" sheetId="1" r:id="rId1"/>
     <sheet name="U = f(R)" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -73,7 +73,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -89,9 +89,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -114,22 +114,22 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="3"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="tx1"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -175,7 +175,7 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>21</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>24.6</c:v>
@@ -232,7 +232,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-47E2-442D-BBE9-231D83BF65A1}"/>
             </c:ext>
@@ -246,11 +246,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="214381744"/>
-        <c:axId val="281596904"/>
+        <c:axId val="291182232"/>
+        <c:axId val="291181840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="214381744"/>
+        <c:axId val="291182232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -290,30 +290,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400" baseline="0">
-                    <a:effectLst/>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
+                  <a:rPr lang="en-US"/>
                   <a:t>U</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="ru-RU" sz="1400" baseline="-25000">
-                    <a:effectLst/>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t>вх</a:t>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>вх, Ом</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="ru-RU" sz="1400" baseline="0">
-                    <a:effectLst/>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t>, Ом</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" sz="1400">
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                </a:endParaRPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -343,7 +327,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -369,7 +353,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -381,15 +365,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="281596904"/>
+        <c:crossAx val="291181840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="281596904"/>
+        <c:axId val="291181840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -416,7 +400,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -429,26 +413,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
-                    <a:effectLst/>
-                  </a:rPr>
+                  <a:rPr lang="en-US"/>
                   <a:t>U</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="ru-RU" sz="1400" b="0" i="0" baseline="-25000">
-                    <a:effectLst/>
-                  </a:rPr>
-                  <a:t>вых</a:t>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>вых, В</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="ru-RU" sz="1400" b="0" i="0" baseline="0">
-                    <a:effectLst/>
-                  </a:rPr>
-                  <a:t>, В</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" sz="1400">
-                  <a:effectLst/>
-                </a:endParaRPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -466,7 +438,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -478,7 +450,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -504,7 +476,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -516,10 +488,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="214381744"/>
+        <c:crossAx val="291182232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -540,7 +512,12 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:noFill/>
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -552,7 +529,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -564,9 +541,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -589,22 +566,22 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="3"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="tx1"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -773,7 +750,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F918-4F91-8FC8-8662D08EC0C7}"/>
             </c:ext>
@@ -787,11 +764,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="214381744"/>
-        <c:axId val="281596904"/>
+        <c:axId val="291183800"/>
+        <c:axId val="291181056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="214381744"/>
+        <c:axId val="291183800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -831,30 +808,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400">
-                    <a:effectLst/>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
+                  <a:rPr lang="en-US"/>
                   <a:t>R</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="ru-RU" sz="1400" baseline="-25000">
-                    <a:effectLst/>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t>н</a:t>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>н, Ом</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="ru-RU" sz="1400" baseline="0">
-                    <a:effectLst/>
-                    <a:latin typeface="+mn-lt"/>
-                  </a:rPr>
-                  <a:t>, Ом</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" sz="1400">
-                  <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
-                </a:endParaRPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -884,7 +845,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -910,7 +871,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -922,15 +883,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="281596904"/>
+        <c:crossAx val="291181056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="281596904"/>
+        <c:axId val="291181056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -957,7 +918,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -970,26 +931,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
-                    <a:effectLst/>
-                  </a:rPr>
+                  <a:rPr lang="en-US"/>
                   <a:t>U</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="ru-RU" sz="1400" b="0" i="0" baseline="-25000">
-                    <a:effectLst/>
-                  </a:rPr>
-                  <a:t>вых</a:t>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>вых, В</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="ru-RU" sz="1400" b="0" i="0" baseline="0">
-                    <a:effectLst/>
-                  </a:rPr>
-                  <a:t>, В</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" sz="1400">
-                  <a:effectLst/>
-                </a:endParaRPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1007,7 +956,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1019,7 +968,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="ru-RU"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1045,7 +994,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1057,10 +1006,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="214381744"/>
+        <c:crossAx val="291183800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1081,7 +1030,12 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:noFill/>
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1093,7 +1047,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1101,6 +1055,408 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12715048118985126"/>
+          <c:y val="0.17171296296296296"/>
+          <c:w val="0.8138425196850394"/>
+          <c:h val="0.66070246427529888"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'U = f(R)'!$C$2:$C$25</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>54.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55.849999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45.023255813953483</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44.603174603174601</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.629489603024574</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21.360631952281153</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.781331638777097</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.212121212121211</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.291827255657672</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.641232806526624</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.8828319978983323</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.8348577746507191</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.1146639739706048</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.7906032852376805</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.6151413058036868</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.8569213356979271</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.5329407557119223</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.2377164540032819</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.1300121782410386</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.8954611260480139</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.8154370361220056</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.0696335197390825</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.4830037468211663</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.0107922360827006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'U = f(R)'!$B$2:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0.54100000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.117</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9359999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.81</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.38</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.41</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.44</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.45</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.45</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.45</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.45</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.45</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.45</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.46</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.47</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.47</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.47</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="293979944"/>
+        <c:axId val="293976808"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="293979944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="293976808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="293976808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="293979944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -1184,6 +1540,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1701,6 +2097,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2285,13 +3197,136 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Диаграмма 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0.3875</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.05</cdr:x>
+      <cdr:y>0.6125</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="16200000">
+          <a:off x="-194310" y="1257300"/>
+          <a:ext cx="617220" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>U</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100"/>
+            <a:t>вых,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100" baseline="0"/>
+            <a:t> В</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.48833</cdr:x>
+      <cdr:y>0.89444</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.6</cdr:x>
+      <cdr:y>0.98611</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2232660" y="2453640"/>
+          <a:ext cx="510540" cy="251460"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>I</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100"/>
+            <a:t>н,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1100" baseline="0"/>
+            <a:t> мА</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2329,7 +3364,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2401,7 +3436,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2578,16 +3613,16 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2595,7 +3630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1.091</v>
       </c>
@@ -2609,7 +3644,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2.98</v>
       </c>
@@ -2623,7 +3658,7 @@
         <v>507.46</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>4.97</v>
       </c>
@@ -2631,7 +3666,7 @@
         <v>3.17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>6.99</v>
       </c>
@@ -2639,7 +3674,7 @@
         <v>4.3499999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>9.0399999999999991</v>
       </c>
@@ -2647,7 +3682,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>11.05</v>
       </c>
@@ -2655,7 +3690,7 @@
         <v>5.23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>13.03</v>
       </c>
@@ -2663,7 +3698,7 @@
         <v>5.33</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>15</v>
       </c>
@@ -2671,7 +3706,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>16.96</v>
       </c>
@@ -2679,7 +3714,7 @@
         <v>5.45</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>19.02</v>
       </c>
@@ -2687,7 +3722,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>21</v>
       </c>
@@ -2695,15 +3730,15 @@
         <v>5.53</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1">
         <v>5.56</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>24.6</v>
       </c>
@@ -2711,39 +3746,39 @@
         <v>5.58</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
     </row>
@@ -2758,12 +3793,12 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="B2" sqref="B2:C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2774,7 +3809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -2786,7 +3821,7 @@
         <v>54.1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>20</v>
       </c>
@@ -2798,7 +3833,7 @@
         <v>55.849999999999994</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>43</v>
       </c>
@@ -2810,7 +3845,7 @@
         <v>45.023255813953483</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>63</v>
       </c>
@@ -2822,7 +3857,7 @@
         <v>44.603174603174601</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>222.18</v>
       </c>
@@ -2834,7 +3869,7 @@
         <v>23.629489603024574</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>248.12</v>
       </c>
@@ -2846,7 +3881,7 @@
         <v>21.360631952281153</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>283.26</v>
       </c>
@@ -2858,7 +3893,7 @@
         <v>18.781331638777097</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>330</v>
       </c>
@@ -2870,7 +3905,7 @@
         <v>16.212121212121211</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>404.76</v>
       </c>
@@ -2882,7 +3917,7 @@
         <v>13.291827255657672</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>507.46</v>
       </c>
@@ -2894,7 +3929,7 @@
         <v>10.641232806526624</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>609.04</v>
       </c>
@@ -2906,7 +3941,7 @@
         <v>8.8828319978983323</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>795.92</v>
       </c>
@@ -2918,7 +3953,7 @@
         <v>6.8348577746507191</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>891.3</v>
       </c>
@@ -2930,7 +3965,7 @@
         <v>6.1146639739706048</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>941.18</v>
       </c>
@@ -2942,7 +3977,7 @@
         <v>5.7906032852376805</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>970.59</v>
       </c>
@@ -2954,7 +3989,7 @@
         <v>5.6151413058036868</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>1122.1099999999999</v>
       </c>
@@ -2966,7 +4001,7 @@
         <v>4.8569213356979271</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>1202.31</v>
       </c>
@@ -2978,7 +4013,7 @@
         <v>4.5329407557119223</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>1286.07</v>
       </c>
@@ -2990,7 +4025,7 @@
         <v>4.2377164540032819</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>1322.03</v>
       </c>
@@ -3002,7 +4037,7 @@
         <v>4.1300121782410386</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>1885.71</v>
       </c>
@@ -3014,7 +4049,7 @@
         <v>2.8954611260480139</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>1942.86</v>
       </c>
@@ -3026,7 +4061,7 @@
         <v>2.8154370361220056</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>2642.98</v>
       </c>
@@ -3038,7 +4073,7 @@
         <v>2.0696335197390825</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>3688.46</v>
       </c>
@@ -3050,7 +4085,7 @@
         <v>1.4830037468211663</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>5421.49</v>
       </c>
@@ -3062,11 +4097,11 @@
         <v>1.0107922360827006</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
     </row>

</xml_diff>